<commit_message>
updated problem statement (typo) and benchmark results
</commit_message>
<xml_diff>
--- a/experiments/benchmark_1/benchmark_processed.xlsx
+++ b/experiments/benchmark_1/benchmark_processed.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\DP\git\experiments\benchmark_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D907B3D-554A-4E07-AD47-A5D1023FD3A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1B24C05-BCE1-424B-90E6-77A781371417}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,12 +30,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Solve time [ms]</t>
-  </si>
-  <si>
-    <t>Environment:</t>
   </si>
   <si>
     <t>g++ (GCC) 8.2.0, optimization flags: -O3 -march=native</t>
@@ -78,10 +75,7 @@
     </r>
   </si>
   <si>
-    <t>Solver:</t>
-  </si>
-  <si>
-    <t>Longest tasks first solver v1.1</t>
+    <t>Longest tasks first solver (with early inner loop exit)</t>
   </si>
 </sst>
 </file>
@@ -706,21 +700,6 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="poly"/>
-            <c:order val="2"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>benchmark!$A$2:$A$101</c:f>
@@ -1401,7 +1380,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="cs-CZ"/>
-                  <a:t>Problem size</a:t>
+                  <a:t>Number of tasks</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -2544,7 +2523,7 @@
   <dimension ref="A1:F101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2555,19 +2534,19 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1000</v>
       </c>
@@ -2579,7 +2558,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="F2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -2594,7 +2573,7 @@
         <v>1.2999999999999999E-2</v>
       </c>
       <c r="F3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -2609,7 +2588,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="F4" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -2623,11 +2602,8 @@
         <f t="shared" si="0"/>
         <v>5.8000000000000003E-2</v>
       </c>
-      <c r="F5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5000</v>
       </c>
@@ -2637,9 +2613,6 @@
       <c r="C6">
         <f t="shared" si="0"/>
         <v>8.4000000000000005E-2</v>
-      </c>
-      <c r="F6" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>